<commit_message>
Removed unecessary files and directories
</commit_message>
<xml_diff>
--- a/STD_test_cases 4 (1).xlsx
+++ b/STD_test_cases 4 (1).xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Desktop\Testing_API_Twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BC82C17-DFB8-4C40-BD04-9D486419407C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C888C0-85FB-45B9-8719-3795C1754C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="96">
   <si>
     <t>Test Case 1</t>
   </si>
@@ -56,12 +45,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>URL,  username and user_id  "header": {
-    "x-rapidapi-host": "twitter154.p.rapidapi.com",
-    "Content-Type": "application/json"
-  }</t>
-  </si>
-  <si>
     <t>Pre-conditions</t>
   </si>
   <si>
@@ -93,9 +76,6 @@
   </si>
   <si>
     <t>Request has been sent</t>
-  </si>
-  <si>
-    <t>With query string for the username and user_id</t>
   </si>
   <si>
     <t>Receive response</t>
@@ -364,12 +344,21 @@
   <si>
     <t>Confirm that the replied_tweet_id in the response matches the values sent in the request</t>
   </si>
+  <si>
+    <t>URL,  Params: username and user_id  "header": {
+    "x-rapidapi-host": "twitter154.p.rapidapi.com",
+    "Content-Type": "application/json"
+  }</t>
+  </si>
+  <si>
+    <t>The test passed, status code is 200</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,19 +569,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,30 +865,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E263"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" customWidth="1"/>
-    <col min="3" max="3" width="63.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" customWidth="1"/>
+    <col min="3" max="3" width="63.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="16.149999999999999">
+    <row r="3" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -908,7 +897,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="16.149999999999999">
+    <row r="4" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -917,1935 +906,1924 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" ht="66">
+    <row r="5" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.149999999999999">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" ht="16.149999999999999">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" ht="16.149999999999999">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="B8" s="8">
         <v>45493</v>
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" ht="16.149999999999999">
+    <row r="9" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="64.900000000000006">
-      <c r="A13" s="7">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16.149999999999999">
+    </row>
+    <row r="14" spans="1:3" ht="178.2" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16.5">
+    </row>
+    <row r="15" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16.5">
+      <c r="C15" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="26">
+        <v>6</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="33">
-      <c r="A17" s="7">
-        <v>5</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>23</v>
-      </c>
       <c r="C17" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="33">
-      <c r="A18" s="26">
-        <v>6</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:5" ht="16.5">
+    <row r="20" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="16.5">
+    <row r="21" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="16.5">
+    <row r="22" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
     </row>
-    <row r="24" spans="1:5" ht="15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:5" ht="15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" ht="15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:5" ht="15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="16.5">
+    <row r="30" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:5" ht="16.5">
+    <row r="31" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C31" s="9"/>
     </row>
-    <row r="32" spans="1:5" ht="114.75">
+    <row r="32" spans="1:5" ht="113.4" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32" s="9"/>
     </row>
-    <row r="33" spans="1:3" ht="16.5">
+    <row r="33" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="9"/>
-    </row>
-    <row r="34" spans="1:3" ht="16.5">
-      <c r="A34" s="4" t="s">
+      <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C34" s="9"/>
-    </row>
-    <row r="35" spans="1:3" ht="16.5">
-      <c r="A35" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="B35" s="8">
         <v>45493</v>
       </c>
       <c r="C35" s="9"/>
     </row>
-    <row r="36" spans="1:3" ht="16.5">
+    <row r="36" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
       <c r="C36" s="9"/>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
     </row>
-    <row r="38" spans="1:3" ht="15">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="33">
+    </row>
+    <row r="40" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>1</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="16.149999999999999">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>2</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16.5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>5</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="26">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16.149999999999999">
+    <row r="46" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="25"/>
       <c r="C46" s="24"/>
     </row>
-    <row r="47" spans="1:3" ht="16.149999999999999">
+    <row r="47" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" ht="16.149999999999999">
+    <row r="48" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:5" ht="16.149999999999999">
+    <row r="49" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:5" ht="16.149999999999999">
+    <row r="50" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
     </row>
-    <row r="57" spans="1:5" ht="16.149999999999999">
+    <row r="57" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C57" s="9"/>
     </row>
-    <row r="58" spans="1:5" ht="16.149999999999999">
+    <row r="58" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C58" s="9"/>
     </row>
-    <row r="59" spans="1:5" ht="66">
+    <row r="59" spans="1:5" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C59" s="9"/>
     </row>
-    <row r="60" spans="1:5" ht="16.149999999999999">
+    <row r="60" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="9"/>
+    </row>
+    <row r="61" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="9"/>
-    </row>
-    <row r="61" spans="1:5" ht="16.149999999999999">
-      <c r="A61" s="4" t="s">
+      <c r="B61" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="9"/>
+    </row>
+    <row r="62" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C61" s="9"/>
-    </row>
-    <row r="62" spans="1:5" ht="16.149999999999999">
-      <c r="A62" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="B62" s="8">
         <v>45493</v>
       </c>
       <c r="C62" s="9"/>
     </row>
-    <row r="63" spans="1:5" ht="16.149999999999999">
+    <row r="63" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
       </c>
       <c r="C63" s="9"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C66" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="64.900000000000006">
+    </row>
+    <row r="67" spans="1:5" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
         <v>1</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="16.149999999999999">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A68" s="7">
         <v>2</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A69" s="7">
         <v>3</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="16.5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A70" s="7">
         <v>4</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A71" s="7">
         <v>5</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A72" s="26">
         <v>6</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="16.5">
+    <row r="74" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A74" s="7"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:5" ht="16.5">
+    <row r="75" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A75" s="7"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:5" ht="16.5">
+    <row r="76" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A76" s="7"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:5" ht="16.5">
+    <row r="77" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="79" spans="1:5" ht="15">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
     </row>
-    <row r="82" spans="1:3" ht="16.5">
+    <row r="82" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A82" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B82" s="16"/>
       <c r="C82" s="16"/>
     </row>
-    <row r="83" spans="1:3" ht="16.5">
+    <row r="83" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
       <c r="B83" s="16"/>
       <c r="C83" s="16"/>
     </row>
-    <row r="84" spans="1:3" ht="33">
+    <row r="84" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A84" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C84" s="16"/>
     </row>
-    <row r="85" spans="1:3" ht="16.5">
+    <row r="85" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A85" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C85" s="16"/>
     </row>
-    <row r="86" spans="1:3" ht="114.75">
+    <row r="86" spans="1:3" ht="113.4" x14ac:dyDescent="0.3">
       <c r="A86" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C86" s="16"/>
     </row>
-    <row r="87" spans="1:3" ht="16.5">
+    <row r="87" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="C87" s="16"/>
+    </row>
+    <row r="88" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A88" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C87" s="16"/>
-    </row>
-    <row r="88" spans="1:3" ht="16.5">
-      <c r="A88" s="17" t="s">
+      <c r="B88" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="16"/>
+    </row>
+    <row r="89" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="C88" s="16"/>
-    </row>
-    <row r="89" spans="1:3" ht="16.5">
-      <c r="A89" s="17" t="s">
-        <v>11</v>
       </c>
       <c r="B89" s="8">
         <v>45493</v>
       </c>
       <c r="C89" s="16"/>
     </row>
-    <row r="90" spans="1:3" ht="16.5">
+    <row r="90" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A90" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B90" s="1">
         <v>1</v>
       </c>
       <c r="C90" s="16"/>
     </row>
-    <row r="91" spans="1:3" ht="15.75">
+    <row r="91" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="18"/>
       <c r="B91" s="18"/>
       <c r="C91" s="18"/>
     </row>
-    <row r="92" spans="1:3" ht="15.75">
+    <row r="92" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="18"/>
       <c r="B92" s="18"/>
       <c r="C92" s="18"/>
     </row>
-    <row r="93" spans="1:3" ht="16.5">
+    <row r="93" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="C93" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C93" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="66">
+    </row>
+    <row r="94" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A94" s="7">
         <v>1</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A95" s="7">
         <v>2</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A96" s="7">
         <v>3</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C96" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="16.5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A97" s="7">
         <v>4</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A98" s="7">
         <v>5</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C98" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A99" s="26">
         <v>6</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C99" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="16.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A100" s="21"/>
     </row>
-    <row r="101" spans="1:5" ht="16.5">
+    <row r="101" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A101" s="21"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:5" ht="16.5">
+    <row r="102" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A102" s="21"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="1:5" ht="16.5">
+    <row r="103" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A103" s="7"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="1:5" ht="16.5">
+    <row r="104" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A104" s="7"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="1:5" ht="16.5">
+    <row r="105" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A105" s="7"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="1:5" ht="15">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="11"/>
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
     </row>
-    <row r="109" spans="1:5" ht="16.5">
+    <row r="109" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A109" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B109" s="16"/>
       <c r="C109" s="16"/>
     </row>
-    <row r="110" spans="1:5" ht="16.5">
+    <row r="110" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A110" s="13"/>
       <c r="B110" s="16"/>
       <c r="C110" s="16"/>
     </row>
-    <row r="111" spans="1:5" ht="33">
+    <row r="111" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A111" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B111" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C111" s="16"/>
     </row>
-    <row r="112" spans="1:5" ht="16.5">
+    <row r="112" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A112" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C112" s="16"/>
     </row>
-    <row r="113" spans="1:3" ht="66">
+    <row r="113" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A113" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C113" s="16"/>
     </row>
-    <row r="114" spans="1:3" ht="33">
+    <row r="114" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A114" s="17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C114" s="16"/>
     </row>
-    <row r="115" spans="1:3" ht="16.5">
+    <row r="115" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A115" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="C115" s="16"/>
+    </row>
+    <row r="116" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A116" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="C115" s="16"/>
-    </row>
-    <row r="116" spans="1:3" ht="16.5">
-      <c r="A116" s="17" t="s">
-        <v>11</v>
       </c>
       <c r="B116" s="8">
         <v>45493</v>
       </c>
       <c r="C116" s="16"/>
     </row>
-    <row r="117" spans="1:3" ht="16.5">
+    <row r="117" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A117" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B117" s="1">
         <v>1</v>
       </c>
       <c r="C117" s="16"/>
     </row>
-    <row r="118" spans="1:3" ht="15.75">
+    <row r="118" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="18"/>
       <c r="B118" s="18"/>
       <c r="C118" s="18"/>
     </row>
-    <row r="119" spans="1:3" ht="15.75">
+    <row r="119" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="18"/>
       <c r="B119" s="18"/>
       <c r="C119" s="18"/>
     </row>
-    <row r="120" spans="1:3" ht="16.5">
+    <row r="120" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A120" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B120" s="20" t="s">
+      <c r="C120" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="49.5">
+    </row>
+    <row r="121" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A121" s="21">
         <v>1</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A122" s="21">
         <v>2</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A123" s="21">
         <v>3</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="16.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A124" s="13">
         <v>4</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C124" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A125" s="13">
         <v>5</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A126" s="21">
         <v>6</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="16.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A127" s="21"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="1:3" ht="16.5">
+    <row r="128" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A128" s="21"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="1:5" ht="16.5">
+    <row r="129" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A129" s="21"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="1:5" ht="16.5">
+    <row r="130" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A130" s="7"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="1:5" ht="16.5">
+    <row r="131" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A131" s="7"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="1:5" ht="16.5">
+    <row r="132" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A132" s="7"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="1:5" ht="15">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="11"/>
       <c r="B133" s="11"/>
       <c r="C133" s="11"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
     </row>
-    <row r="136" spans="1:5" ht="16.5">
+    <row r="136" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A136" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B136" s="16"/>
       <c r="C136" s="16"/>
     </row>
-    <row r="137" spans="1:5" ht="16.5">
+    <row r="137" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A137" s="13"/>
       <c r="B137" s="16"/>
       <c r="C137" s="16"/>
     </row>
-    <row r="138" spans="1:5" ht="33">
+    <row r="138" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A138" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C138" s="16"/>
     </row>
-    <row r="139" spans="1:5" ht="33">
+    <row r="139" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A139" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C139" s="16"/>
     </row>
-    <row r="140" spans="1:5" ht="66">
+    <row r="140" spans="1:5" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A140" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C140" s="16"/>
     </row>
-    <row r="141" spans="1:5" ht="16.5">
+    <row r="141" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A141" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="C141" s="16"/>
+    </row>
+    <row r="142" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A142" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C141" s="16"/>
-    </row>
-    <row r="142" spans="1:5" ht="16.5">
-      <c r="A142" s="17" t="s">
+      <c r="B142" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="C142" s="16"/>
+    </row>
+    <row r="143" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A143" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="C142" s="16"/>
-    </row>
-    <row r="143" spans="1:5" ht="16.5">
-      <c r="A143" s="17" t="s">
-        <v>11</v>
       </c>
       <c r="B143" s="8">
         <v>45493</v>
       </c>
       <c r="C143" s="16"/>
     </row>
-    <row r="144" spans="1:5" ht="16.5">
+    <row r="144" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A144" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B144" s="1">
         <v>1</v>
       </c>
       <c r="C144" s="16"/>
     </row>
-    <row r="145" spans="1:5" ht="15.75">
+    <row r="145" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="18"/>
       <c r="B145" s="18"/>
       <c r="C145" s="18"/>
     </row>
-    <row r="146" spans="1:5" ht="15.75">
+    <row r="146" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="18"/>
       <c r="B146" s="18"/>
       <c r="C146" s="18"/>
     </row>
-    <row r="147" spans="1:5" ht="16.5">
+    <row r="147" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A147" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B147" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B147" s="20" t="s">
+      <c r="C147" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C147" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="30.75">
+    </row>
+    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>1</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="49.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A149" s="21">
         <v>2</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A150" s="21">
         <v>3</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C150" s="27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="32.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A151" s="13">
         <v>4</v>
       </c>
       <c r="B151" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C151" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="16.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A152" s="13">
         <v>5</v>
       </c>
       <c r="B152" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C152" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A153" s="21">
         <v>6</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A154" s="21">
         <v>7</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" ht="16.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A155" s="21"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="1:5" ht="16.5">
+    <row r="156" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A156" s="21"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="1:5" ht="16.5">
+    <row r="157" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A157" s="7"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="1:5" ht="16.5">
+    <row r="158" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A158" s="7"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="1:5" ht="16.5">
+    <row r="159" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A159" s="7"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="1:5" ht="15">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="11"/>
       <c r="B160" s="11"/>
       <c r="C160" s="11"/>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
     </row>
-    <row r="163" spans="1:3" ht="16.5">
+    <row r="163" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A163" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B163" s="22"/>
       <c r="C163" s="22"/>
     </row>
-    <row r="164" spans="1:3" ht="16.5">
+    <row r="164" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A164" s="13"/>
       <c r="B164" s="22"/>
       <c r="C164" s="22"/>
     </row>
-    <row r="165" spans="1:3" ht="33">
+    <row r="165" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A165" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B165" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C165" s="22"/>
     </row>
-    <row r="166" spans="1:3" ht="16.5">
+    <row r="166" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A166" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C166" s="22"/>
     </row>
-    <row r="167" spans="1:3" ht="82.5">
+    <row r="167" spans="1:3" ht="81" x14ac:dyDescent="0.35">
       <c r="A167" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C167" s="22"/>
     </row>
-    <row r="168" spans="1:3" ht="16.5">
+    <row r="168" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A168" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B168" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="C168" s="22"/>
+    </row>
+    <row r="169" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A169" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C168" s="22"/>
-    </row>
-    <row r="169" spans="1:3" ht="16.5">
-      <c r="A169" s="17" t="s">
+      <c r="B169" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="C169" s="22"/>
+    </row>
+    <row r="170" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A170" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="C169" s="22"/>
-    </row>
-    <row r="170" spans="1:3" ht="16.5">
-      <c r="A170" s="17" t="s">
-        <v>11</v>
       </c>
       <c r="B170" s="8">
         <v>45493</v>
       </c>
       <c r="C170" s="22"/>
     </row>
-    <row r="171" spans="1:3" ht="16.5">
+    <row r="171" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A171" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B171" s="1">
         <v>1</v>
       </c>
       <c r="C171" s="22"/>
     </row>
-    <row r="172" spans="1:3" ht="16.5">
+    <row r="172" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A172" s="14"/>
       <c r="B172" s="14"/>
       <c r="C172" s="14"/>
     </row>
-    <row r="173" spans="1:3" ht="16.5">
+    <row r="173" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A173" s="14"/>
       <c r="B173" s="14"/>
       <c r="C173" s="14"/>
     </row>
-    <row r="174" spans="1:3" ht="16.5">
+    <row r="174" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A174" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B174" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B174" s="20" t="s">
+      <c r="C174" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C174" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="66">
+    </row>
+    <row r="175" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A175" s="21">
         <v>1</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A176" s="21">
         <v>2</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A177" s="21">
         <v>3</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C177" s="27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" ht="16.5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A178" s="13">
         <v>4</v>
       </c>
       <c r="B178" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C178" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A179" s="13">
         <v>5</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C179" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" ht="49.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A180" s="21">
         <v>6</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C180" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A181" s="21">
         <v>7</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C181" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" ht="16.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A182" s="21"/>
       <c r="B182" s="14"/>
       <c r="C182" s="14"/>
     </row>
-    <row r="183" spans="1:5" ht="16.5">
+    <row r="183" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A183" s="21"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
     </row>
-    <row r="184" spans="1:5" ht="16.5">
+    <row r="184" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A184" s="21"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
     </row>
-    <row r="185" spans="1:5" ht="16.5">
+    <row r="185" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A185" s="7"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
     </row>
-    <row r="186" spans="1:5" ht="16.5">
+    <row r="186" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A186" s="7"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
     </row>
-    <row r="187" spans="1:5" ht="15">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="11"/>
       <c r="B187" s="11"/>
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="11"/>
     </row>
-    <row r="190" spans="1:5" ht="16.5">
+    <row r="190" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A190" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B190" s="22"/>
       <c r="C190" s="22"/>
     </row>
-    <row r="191" spans="1:5" ht="16.5">
+    <row r="191" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A191" s="13"/>
       <c r="B191" s="22"/>
       <c r="C191" s="22"/>
     </row>
-    <row r="192" spans="1:5" ht="33">
+    <row r="192" spans="1:5" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A192" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B192" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C192" s="22"/>
     </row>
-    <row r="193" spans="1:3" ht="16.5">
+    <row r="193" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A193" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C193" s="22"/>
     </row>
-    <row r="194" spans="1:3" ht="66">
+    <row r="194" spans="1:3" ht="64.8" x14ac:dyDescent="0.35">
       <c r="A194" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C194" s="22"/>
     </row>
-    <row r="195" spans="1:3" ht="16.5">
+    <row r="195" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A195" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B195" s="1" t="s">
+      <c r="C195" s="22"/>
+    </row>
+    <row r="196" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A196" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C195" s="22"/>
-    </row>
-    <row r="196" spans="1:3" ht="16.5">
-      <c r="A196" s="17" t="s">
+      <c r="B196" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="C196" s="22"/>
+    </row>
+    <row r="197" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A197" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="C196" s="22"/>
-    </row>
-    <row r="197" spans="1:3" ht="16.5">
-      <c r="A197" s="17" t="s">
-        <v>11</v>
       </c>
       <c r="B197" s="8">
         <v>45493</v>
       </c>
       <c r="C197" s="22"/>
     </row>
-    <row r="198" spans="1:3" ht="16.5">
+    <row r="198" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A198" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B198" s="1">
         <v>1</v>
       </c>
       <c r="C198" s="22"/>
     </row>
-    <row r="199" spans="1:3" ht="16.5">
+    <row r="199" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A199" s="14"/>
       <c r="B199" s="14"/>
       <c r="C199" s="14"/>
     </row>
-    <row r="200" spans="1:3" ht="16.5">
+    <row r="200" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A200" s="14"/>
       <c r="B200" s="14"/>
       <c r="C200" s="14"/>
     </row>
-    <row r="201" spans="1:3" ht="16.5">
+    <row r="201" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A201" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B201" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B201" s="20" t="s">
+      <c r="C201" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C201" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="49.5">
+    </row>
+    <row r="202" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A202" s="21">
         <v>1</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A203" s="21">
         <v>2</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A204" s="21">
         <v>3</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C204" s="27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="16.5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A205" s="13">
         <v>4</v>
       </c>
       <c r="B205" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C205" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A206" s="13">
         <v>5</v>
       </c>
       <c r="B206" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C206" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A207" s="21">
         <v>6</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="16.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A208" s="21"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
     </row>
-    <row r="209" spans="1:5" ht="16.5">
+    <row r="209" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A209" s="21"/>
       <c r="B209" s="14"/>
       <c r="C209" s="14"/>
     </row>
-    <row r="210" spans="1:5" ht="16.5">
+    <row r="210" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A210" s="21"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
     </row>
-    <row r="211" spans="1:5" ht="16.5">
+    <row r="211" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A211" s="21"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
     </row>
-    <row r="212" spans="1:5" ht="16.5">
+    <row r="212" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A212" s="7"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
     </row>
-    <row r="213" spans="1:5" ht="16.5">
+    <row r="213" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A213" s="7"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
     </row>
-    <row r="214" spans="1:5" ht="15">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="11"/>
       <c r="B214" s="11"/>
       <c r="C214" s="11"/>
       <c r="D214" s="11"/>
       <c r="E214" s="11"/>
     </row>
-    <row r="217" spans="1:5" ht="16.5">
+    <row r="217" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A217" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B217" s="22"/>
       <c r="C217" s="22"/>
     </row>
-    <row r="218" spans="1:5" ht="16.5">
+    <row r="218" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A218" s="13"/>
       <c r="B218" s="22"/>
       <c r="C218" s="22"/>
     </row>
-    <row r="219" spans="1:5" ht="33">
+    <row r="219" spans="1:5" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A219" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B219" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C219" s="22"/>
     </row>
-    <row r="220" spans="1:5" ht="33">
+    <row r="220" spans="1:5" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A220" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C220" s="22"/>
     </row>
-    <row r="221" spans="1:5" ht="114.75">
+    <row r="221" spans="1:5" ht="113.4" x14ac:dyDescent="0.35">
       <c r="A221" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C221" s="22"/>
     </row>
-    <row r="222" spans="1:5" ht="16.5">
+    <row r="222" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A222" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B222" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="C222" s="22"/>
+    </row>
+    <row r="223" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A223" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C222" s="22"/>
-    </row>
-    <row r="223" spans="1:5" ht="16.5">
-      <c r="A223" s="17" t="s">
+      <c r="B223" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="C223" s="22"/>
+    </row>
+    <row r="224" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A224" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="C223" s="22"/>
-    </row>
-    <row r="224" spans="1:5" ht="16.5">
-      <c r="A224" s="17" t="s">
-        <v>11</v>
       </c>
       <c r="B224" s="8">
         <v>45493</v>
       </c>
       <c r="C224" s="22"/>
     </row>
-    <row r="225" spans="1:3" ht="16.5">
+    <row r="225" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A225" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B225" s="1">
         <v>1</v>
       </c>
       <c r="C225" s="22"/>
     </row>
-    <row r="226" spans="1:3" ht="16.5">
+    <row r="226" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A226" s="14"/>
       <c r="B226" s="14"/>
       <c r="C226" s="14"/>
     </row>
-    <row r="227" spans="1:3" ht="16.5">
+    <row r="227" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A227" s="14"/>
       <c r="B227" s="14"/>
       <c r="C227" s="14"/>
     </row>
-    <row r="228" spans="1:3" ht="16.5">
+    <row r="228" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A228" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B228" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B228" s="20" t="s">
+      <c r="C228" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C228" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="33">
+    </row>
+    <row r="229" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A229" s="21">
         <v>1</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="49.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A230" s="21">
         <v>2</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A231" s="23">
         <v>3</v>
       </c>
       <c r="B231" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C231" s="28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="16.5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A232" s="21">
         <v>4</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C232" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A233" s="13">
         <v>5</v>
       </c>
       <c r="B233" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C233" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A234" s="13">
         <v>6</v>
       </c>
       <c r="B234" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C234" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="16.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A235" s="21"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
     </row>
-    <row r="236" spans="1:3" ht="16.5">
+    <row r="236" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A236" s="21"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
     </row>
-    <row r="237" spans="1:3" ht="16.5">
+    <row r="237" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A237" s="21"/>
       <c r="B237" s="14"/>
       <c r="C237" s="14"/>
     </row>
-    <row r="238" spans="1:3" ht="16.5">
+    <row r="238" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A238" s="21"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
     </row>
-    <row r="239" spans="1:3" ht="16.5">
+    <row r="239" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A239" s="7"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
     </row>
-    <row r="240" spans="1:3" ht="16.5">
+    <row r="240" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A240" s="7"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
     </row>
-    <row r="241" spans="1:5" ht="15">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="11"/>
       <c r="B241" s="11"/>
       <c r="C241" s="11"/>
       <c r="D241" s="11"/>
       <c r="E241" s="11"/>
     </row>
-    <row r="244" spans="1:5" ht="15.75">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B244" s="9"/>
       <c r="C244" s="9"/>
     </row>
-    <row r="245" spans="1:5" ht="15">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="3"/>
       <c r="B245" s="9"/>
       <c r="C245" s="9"/>
     </row>
-    <row r="246" spans="1:5" ht="16.5">
+    <row r="246" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A246" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B246" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C246" s="9"/>
     </row>
-    <row r="247" spans="1:5" ht="16.5">
+    <row r="247" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A247" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C247" s="9"/>
     </row>
-    <row r="248" spans="1:5" ht="82.5">
+    <row r="248" spans="1:5" ht="81" x14ac:dyDescent="0.3">
       <c r="A248" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C248" s="9"/>
     </row>
-    <row r="249" spans="1:5" ht="16.5">
+    <row r="249" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B249" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B249" s="1" t="s">
+      <c r="C249" s="9"/>
+    </row>
+    <row r="250" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A250" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C249" s="9"/>
-    </row>
-    <row r="250" spans="1:5" ht="16.5">
-      <c r="A250" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="B250" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C250" s="9"/>
     </row>
-    <row r="251" spans="1:5" ht="16.5">
+    <row r="251" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A251" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B251" s="8">
         <v>45493</v>
       </c>
       <c r="C251" s="9"/>
     </row>
-    <row r="252" spans="1:5" ht="16.5">
+    <row r="252" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A252" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B252" s="1">
         <v>1</v>
       </c>
       <c r="C252" s="9"/>
     </row>
-    <row r="253" spans="1:5" ht="15">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="10"/>
       <c r="B253" s="10"/>
       <c r="C253" s="10"/>
     </row>
-    <row r="254" spans="1:5" ht="15">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="10"/>
       <c r="B254" s="10"/>
       <c r="C254" s="10"/>
     </row>
-    <row r="255" spans="1:5" ht="15.75">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B255" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B255" s="6" t="s">
+      <c r="C255" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C255" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5" ht="49.5">
+    </row>
+    <row r="256" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A256" s="7">
         <v>1</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A257" s="7">
         <v>2</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" ht="16.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A258" s="7">
         <v>3</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C258" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" ht="16.5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A259" s="7">
         <v>4</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C259" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" ht="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A260" s="7">
         <v>5</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C260" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3" ht="16.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A261" s="7">
         <v>6</v>
       </c>
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
     </row>
-    <row r="262" spans="1:3" ht="16.5">
+    <row r="262" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A262" s="7">
         <v>7</v>
       </c>
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
     </row>
-    <row r="263" spans="1:3" ht="16.5">
+    <row r="263" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A263" s="7">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Added a test for the tweet details to check the text itself
</commit_message>
<xml_diff>
--- a/STD_test_cases 4 (1).xlsx
+++ b/STD_test_cases 4 (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Desktop\Testing_API_Twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C888C0-85FB-45B9-8719-3795C1754C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1318855-5E98-4230-B0A0-19DF1C84E1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,12 +174,6 @@
     <t>To validate retrieving tweet details from the API</t>
   </si>
   <si>
-    <t>URL,  tweet_id and expected_tweet_id   "header": {
-    "x-rapidapi-host": "twitter154.p.rapidapi.com",
-    "Content-Type": "application/json"
-  }</t>
-  </si>
-  <si>
     <t>API endpoint, configuration file with tweet_id and expected_tweet_id</t>
   </si>
   <si>
@@ -352,6 +346,62 @@
   </si>
   <si>
     <t>The test passed, status code is 200</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Assistant"/>
+      </rPr>
+      <t>URL,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Assistant"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Assistant"/>
+      </rPr>
+      <t>Params:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Assistant"/>
+      </rPr>
+      <t xml:space="preserve"> "tweet_id" and "expected_tweet_id"   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Assistant"/>
+      </rPr>
+      <t>"header":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Assistant"/>
+      </rPr>
+      <t xml:space="preserve"> {
+    "x-rapidapi-host": "twitter154.p.rapidapi.com",
+    "Content-Type": "application/json"
+  }</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -865,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="9"/>
     </row>
@@ -1002,7 +1052,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
@@ -1681,12 +1731,12 @@
       </c>
       <c r="C112" s="16"/>
     </row>
-    <row r="113" spans="1:3" ht="64.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="81" x14ac:dyDescent="0.3">
       <c r="A113" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="C113" s="16"/>
     </row>
@@ -1695,7 +1745,7 @@
         <v>6</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C114" s="16"/>
     </row>
@@ -1752,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>16</v>
@@ -1763,7 +1813,7 @@
         <v>2</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>16</v>
@@ -1777,7 +1827,7 @@
         <v>17</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -1785,7 +1835,7 @@
         <v>4</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C124" s="18" t="s">
         <v>20</v>
@@ -1796,7 +1846,7 @@
         <v>5</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C125" s="14" t="s">
         <v>20</v>
@@ -1807,7 +1857,7 @@
         <v>6</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>20</v>
@@ -1852,7 +1902,7 @@
     </row>
     <row r="136" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A136" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B136" s="16"/>
       <c r="C136" s="16"/>
@@ -1867,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C138" s="16"/>
     </row>
@@ -1876,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C139" s="16"/>
     </row>
@@ -1885,7 +1935,7 @@
         <v>5</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C140" s="16"/>
     </row>
@@ -1951,10 +2001,10 @@
         <v>1</v>
       </c>
       <c r="B148" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C148" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="C148" s="10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
@@ -1962,7 +2012,7 @@
         <v>2</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>16</v>
@@ -1976,7 +2026,7 @@
         <v>17</v>
       </c>
       <c r="C150" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
@@ -1984,10 +2034,10 @@
         <v>4</v>
       </c>
       <c r="B151" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C151" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="C151" s="18" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
@@ -1995,7 +2045,7 @@
         <v>5</v>
       </c>
       <c r="B152" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C152" s="18" t="s">
         <v>20</v>
@@ -2006,7 +2056,7 @@
         <v>6</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C153" s="14" t="s">
         <v>20</v>
@@ -2017,7 +2067,7 @@
         <v>7</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>20</v>
@@ -2057,7 +2107,7 @@
     </row>
     <row r="163" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A163" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B163" s="22"/>
       <c r="C163" s="22"/>
@@ -2072,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C165" s="22"/>
     </row>
@@ -2081,7 +2131,7 @@
         <v>3</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C166" s="22"/>
     </row>
@@ -2090,7 +2140,7 @@
         <v>5</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C167" s="22"/>
     </row>
@@ -2156,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>16</v>
@@ -2167,7 +2217,7 @@
         <v>2</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>16</v>
@@ -2181,7 +2231,7 @@
         <v>17</v>
       </c>
       <c r="C177" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
@@ -2189,7 +2239,7 @@
         <v>4</v>
       </c>
       <c r="B178" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C178" s="18" t="s">
         <v>20</v>
@@ -2200,7 +2250,7 @@
         <v>5</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C179" s="18" t="s">
         <v>20</v>
@@ -2211,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C180" s="18" t="s">
         <v>20</v>
@@ -2222,7 +2272,7 @@
         <v>7</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C181" s="18" t="s">
         <v>20</v>
@@ -2262,7 +2312,7 @@
     </row>
     <row r="190" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A190" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B190" s="22"/>
       <c r="C190" s="22"/>
@@ -2277,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="B192" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C192" s="22"/>
     </row>
@@ -2286,7 +2336,7 @@
         <v>3</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C193" s="22"/>
     </row>
@@ -2295,7 +2345,7 @@
         <v>5</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C194" s="22"/>
     </row>
@@ -2361,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>16</v>
@@ -2372,7 +2422,7 @@
         <v>2</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>16</v>
@@ -2386,7 +2436,7 @@
         <v>17</v>
       </c>
       <c r="C204" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
@@ -2394,7 +2444,7 @@
         <v>4</v>
       </c>
       <c r="B205" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C205" s="14" t="s">
         <v>20</v>
@@ -2405,7 +2455,7 @@
         <v>5</v>
       </c>
       <c r="B206" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C206" s="14" t="s">
         <v>20</v>
@@ -2416,7 +2466,7 @@
         <v>6</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>20</v>
@@ -2461,7 +2511,7 @@
     </row>
     <row r="217" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A217" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B217" s="22"/>
       <c r="C217" s="22"/>
@@ -2476,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="B219" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C219" s="22"/>
     </row>
@@ -2485,7 +2535,7 @@
         <v>3</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C220" s="22"/>
     </row>
@@ -2494,7 +2544,7 @@
         <v>5</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C221" s="22"/>
     </row>
@@ -2560,10 +2610,10 @@
         <v>1</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="48.6" x14ac:dyDescent="0.3">
@@ -2571,7 +2621,7 @@
         <v>2</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>16</v>
@@ -2585,7 +2635,7 @@
         <v>17</v>
       </c>
       <c r="C231" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -2593,7 +2643,7 @@
         <v>4</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C232" t="s">
         <v>20</v>
@@ -2604,7 +2654,7 @@
         <v>5</v>
       </c>
       <c r="B233" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C233" t="s">
         <v>20</v>
@@ -2615,7 +2665,7 @@
         <v>6</v>
       </c>
       <c r="B234" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C234" t="s">
         <v>20</v>
@@ -2675,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="B246" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C246" s="9"/>
     </row>
@@ -2684,7 +2734,7 @@
         <v>3</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C247" s="9"/>
     </row>
@@ -2693,7 +2743,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C248" s="9"/>
     </row>
@@ -2711,7 +2761,7 @@
         <v>8</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C250" s="9"/>
     </row>
@@ -2759,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>16</v>
@@ -2770,7 +2820,7 @@
         <v>2</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>16</v>
@@ -2784,7 +2834,7 @@
         <v>17</v>
       </c>
       <c r="C258" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -2792,7 +2842,7 @@
         <v>4</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C259" t="s">
         <v>20</v>
@@ -2803,7 +2853,7 @@
         <v>5</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C260" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Updaed the logic in the api tweet details
</commit_message>
<xml_diff>
--- a/STD_test_cases 4 (1).xlsx
+++ b/STD_test_cases 4 (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Desktop\Testing_API_Twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1318855-5E98-4230-B0A0-19DF1C84E1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F30612-E9C8-4BF1-96CB-63634775539D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>Object is created</t>
-  </si>
-  <si>
-    <t>Send a POST request to the API endpoint https://twitter154.p.rapidapi.com/tweet/details with valid headers and tweet details</t>
   </si>
   <si>
     <t>Create an instance of APITweetDetails with the API request</t>
@@ -402,6 +399,9 @@
     "Content-Type": "application/json"
   }</t>
     </r>
+  </si>
+  <si>
+    <t>Send a GET request to the API endpoint https://twitter154.p.rapidapi.com/tweet/details with valid headers and tweet details</t>
   </si>
 </sst>
 </file>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="9"/>
     </row>
@@ -1052,7 +1052,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="32.4" x14ac:dyDescent="0.3">
@@ -1736,7 +1736,7 @@
         <v>5</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C113" s="16"/>
     </row>
@@ -2012,7 +2012,7 @@
         <v>2</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>16</v>
@@ -2034,10 +2034,10 @@
         <v>4</v>
       </c>
       <c r="B151" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C151" s="18" t="s">
         <v>58</v>
-      </c>
-      <c r="C151" s="18" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
@@ -2107,7 +2107,7 @@
     </row>
     <row r="163" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A163" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B163" s="22"/>
       <c r="C163" s="22"/>
@@ -2122,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C165" s="22"/>
     </row>
@@ -2131,7 +2131,7 @@
         <v>3</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C166" s="22"/>
     </row>
@@ -2140,7 +2140,7 @@
         <v>5</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C167" s="22"/>
     </row>
@@ -2206,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>16</v>
@@ -2217,7 +2217,7 @@
         <v>2</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>16</v>
@@ -2231,7 +2231,7 @@
         <v>17</v>
       </c>
       <c r="C177" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
@@ -2250,7 +2250,7 @@
         <v>5</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C179" s="18" t="s">
         <v>20</v>
@@ -2261,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C180" s="18" t="s">
         <v>20</v>
@@ -2272,7 +2272,7 @@
         <v>7</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C181" s="18" t="s">
         <v>20</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="190" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A190" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B190" s="22"/>
       <c r="C190" s="22"/>
@@ -2327,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="B192" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C192" s="22"/>
     </row>
@@ -2336,7 +2336,7 @@
         <v>3</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C193" s="22"/>
     </row>
@@ -2345,7 +2345,7 @@
         <v>5</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C194" s="22"/>
     </row>
@@ -2411,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>16</v>
@@ -2422,7 +2422,7 @@
         <v>2</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>16</v>
@@ -2436,7 +2436,7 @@
         <v>17</v>
       </c>
       <c r="C204" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
@@ -2455,7 +2455,7 @@
         <v>5</v>
       </c>
       <c r="B206" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C206" s="14" t="s">
         <v>20</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="217" spans="1:5" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A217" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B217" s="22"/>
       <c r="C217" s="22"/>
@@ -2526,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="B219" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C219" s="22"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>3</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C220" s="22"/>
     </row>
@@ -2544,7 +2544,7 @@
         <v>5</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C221" s="22"/>
     </row>
@@ -2610,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>56</v>
@@ -2621,7 +2621,7 @@
         <v>2</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>16</v>
@@ -2635,7 +2635,7 @@
         <v>17</v>
       </c>
       <c r="C231" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -2654,7 +2654,7 @@
         <v>5</v>
       </c>
       <c r="B233" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C233" t="s">
         <v>20</v>
@@ -2725,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="B246" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C246" s="9"/>
     </row>
@@ -2734,7 +2734,7 @@
         <v>3</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C247" s="9"/>
     </row>
@@ -2743,7 +2743,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C248" s="9"/>
     </row>
@@ -2761,7 +2761,7 @@
         <v>8</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C250" s="9"/>
     </row>
@@ -2809,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>16</v>
@@ -2820,7 +2820,7 @@
         <v>2</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>16</v>
@@ -2834,7 +2834,7 @@
         <v>17</v>
       </c>
       <c r="C258" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -2853,7 +2853,7 @@
         <v>5</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C260" t="s">
         <v>20</v>

</xml_diff>